<commit_message>
realization download excel with disable field
</commit_message>
<xml_diff>
--- a/export/realizationForm.xlsx
+++ b/export/realizationForm.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="775" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="775"/>
   </bookViews>
   <sheets>
-    <sheet name="Realisasi" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Realisasi" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -81,11 +80,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="YYYY\-MM\-DD"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -94,22 +92,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -123,8 +106,15 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -143,115 +133,103 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
-      <right style="hair"/>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="hair"/>
-      <right style="hair"/>
-      <top style="hair"/>
-      <bottom style="double"/>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
-      <right style="hair"/>
-      <top style="hair"/>
-      <bottom style="hair"/>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="hair"/>
-      <right style="hair"/>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+  </cellStyleXfs>
+  <cellXfs count="10">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-  </cellStyleXfs>
-  <cellXfs count="9">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -310,45 +288,333 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF3C3C3C"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
   <dimension ref="A1:P13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P17" activeCellId="0" sqref="P17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.72959183673469"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.6071428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="100.775510204082"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.3622448979592"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.2551020408163"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.2295918367347"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.4132653061225"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.030612244898"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="14.4438775510204"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.6683673469388"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="17.5051020408163"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="20.0051020408163"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="22.2295918367347"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="24.0357142857143"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="67.6683673469388"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="34.7295918367347"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="8.72959183673469"/>
+    <col min="1" max="1" width="8.7109375"/>
+    <col min="2" max="2" width="30.5703125"/>
+    <col min="3" max="3" width="100.7109375"/>
+    <col min="4" max="4" width="11.5703125"/>
+    <col min="5" max="5" width="17.42578125"/>
+    <col min="6" max="6" width="21.28515625"/>
+    <col min="7" max="7" width="22.28515625"/>
+    <col min="8" max="8" width="10.42578125"/>
+    <col min="9" max="9" width="14"/>
+    <col min="10" max="10" width="14.42578125"/>
+    <col min="11" max="11" width="21.7109375"/>
+    <col min="12" max="12" width="17.5703125"/>
+    <col min="13" max="13" width="20"/>
+    <col min="14" max="14" width="22.28515625"/>
+    <col min="15" max="15" width="24" style="1"/>
+    <col min="16" max="16" width="67.7109375" style="1"/>
+    <col min="17" max="17" width="34.7109375"/>
+    <col min="18" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="63.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:16" ht="63.75" customHeight="1" thickBot="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -367,7 +633,7 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="9" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="3" t="s">
@@ -398,57 +664,52 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:16" ht="13.5" thickTop="1">
       <c r="P2" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:16">
       <c r="P3" s="5"/>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:16">
       <c r="P4" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:16">
       <c r="P5" s="5"/>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:16">
       <c r="P6" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:16">
       <c r="P7" s="5"/>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:16">
       <c r="P8" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:16">
       <c r="P9" s="7"/>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:16">
       <c r="P10" s="7"/>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:16">
       <c r="P11" s="7"/>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:16">
       <c r="P12" s="8"/>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:16">
       <c r="P13" s="5"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>